<commit_message>
Moved files- Trxn map
</commit_message>
<xml_diff>
--- a/Cust-Trxn-Channel-Charts/V2_Charts/dataframe-bargraph-tmp.xlsx
+++ b/Cust-Trxn-Channel-Charts/V2_Charts/dataframe-bargraph-tmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Value</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Level</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -474,6 +479,9 @@
       <c r="D2" t="n">
         <v>1770000</v>
       </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,6 +502,9 @@
       <c r="D3" t="n">
         <v>11200000</v>
       </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,6 +525,9 @@
       <c r="D4" t="n">
         <v>10393000</v>
       </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,6 +548,9 @@
       <c r="D5" t="n">
         <v>2735000</v>
       </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +571,9 @@
       <c r="D6" t="n">
         <v>637000</v>
       </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -574,6 +594,9 @@
       <c r="D7" t="n">
         <v>726000</v>
       </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -594,6 +617,9 @@
       <c r="D8" t="n">
         <v>102000</v>
       </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -614,6 +640,9 @@
       <c r="D9" t="n">
         <v>2960</v>
       </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -634,6 +663,9 @@
       <c r="D10" t="n">
         <v>388</v>
       </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -654,6 +686,9 @@
       <c r="D11" t="n">
         <v>4474000</v>
       </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -674,6 +709,9 @@
       <c r="D12" t="n">
         <v>1241000</v>
       </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -694,6 +732,9 @@
       <c r="D13" t="n">
         <v>209000</v>
       </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -714,6 +755,9 @@
       <c r="D14" t="n">
         <v>205000</v>
       </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -734,6 +778,9 @@
       <c r="D15" t="n">
         <v>155000</v>
       </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -754,6 +801,9 @@
       <c r="D16" t="n">
         <v>124000</v>
       </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -774,6 +824,9 @@
       <c r="D17" t="n">
         <v>58000</v>
       </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -794,6 +847,9 @@
       <c r="D18" t="n">
         <v>843000</v>
       </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -814,6 +870,9 @@
       <c r="D19" t="n">
         <v>678000</v>
       </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -828,12 +887,15 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Icm Technology Handled</t>
+          <t>ICM Technology Handled</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>2630000</v>
       </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -848,12 +910,15 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Nonivr Technology</t>
+          <t>NonIVR Technology</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>29000</v>
       </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -868,12 +933,15 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Transferred Calls</t>
+          <t>Transferred calls</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>3918000</v>
       </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -894,6 +962,9 @@
       <c r="D23" t="n">
         <v>267000</v>
       </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -914,6 +985,9 @@
       <c r="D24" t="n">
         <v>1341000</v>
       </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -934,6 +1008,9 @@
       <c r="D25" t="n">
         <v>691000</v>
       </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -954,6 +1031,9 @@
       <c r="D26" t="n">
         <v>374000</v>
       </c>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -974,6 +1054,9 @@
       <c r="D27" t="n">
         <v>133000</v>
       </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -994,6 +1077,9 @@
       <c r="D28" t="n">
         <v>171000</v>
       </c>
+      <c r="E28" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1008,12 +1094,15 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bcsc (Business Customer Service Center)</t>
+          <t>BCSC (Business Customer Service Center)</t>
         </is>
       </c>
       <c r="D29" t="n">
         <v>466000</v>
       </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1034,6 +1123,9 @@
       <c r="D30" t="n">
         <v>449000</v>
       </c>
+      <c r="E30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1054,6 +1146,9 @@
       <c r="D31" t="n">
         <v>246000</v>
       </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1074,6 +1169,9 @@
       <c r="D32" t="n">
         <v>256000</v>
       </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1094,6 +1192,9 @@
       <c r="D33" t="n">
         <v>137000</v>
       </c>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1114,6 +1215,9 @@
       <c r="D34" t="n">
         <v>479000</v>
       </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1134,6 +1238,9 @@
       <c r="D35" t="n">
         <v>220000</v>
       </c>
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1154,6 +1261,9 @@
       <c r="D36" t="n">
         <v>123000</v>
       </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1174,6 +1284,9 @@
       <c r="D37" t="n">
         <v>136000</v>
       </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1194,6 +1307,9 @@
       <c r="D38" t="n">
         <v>3633827</v>
       </c>
+      <c r="E38" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1214,6 +1330,9 @@
       <c r="D39" t="n">
         <v>24316220</v>
       </c>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1228,12 +1347,15 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Billing &gt; Viewbillcurrentpdf</t>
+          <t>Billing &gt; ViewBillCurrentPDF</t>
         </is>
       </c>
       <c r="D40" t="n">
         <v>8992263</v>
       </c>
+      <c r="E40" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1248,12 +1370,15 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Billing &gt; Viewbillcurrentpdf Historical</t>
+          <t>Billing &gt; ViewBillCurrentPDF historical</t>
         </is>
       </c>
       <c r="D41" t="n">
         <v>9361207</v>
       </c>
+      <c r="E41" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1268,12 +1393,15 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Usage And Rates &gt; View Usage</t>
+          <t>Usage and Rates &gt; View Usage</t>
         </is>
       </c>
       <c r="D42" t="n">
         <v>3193489</v>
       </c>
+      <c r="E42" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1288,12 +1416,15 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Usage And Rates &gt; Compare My Bills</t>
+          <t>Usage and Rates &gt; Compare My Bills</t>
         </is>
       </c>
       <c r="D43" t="n">
         <v>2735761</v>
       </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1308,12 +1439,15 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Usage And Rates &gt; Rate Comparison</t>
+          <t>Usage and Rates &gt; Rate Comparison</t>
         </is>
       </c>
       <c r="D44" t="n">
         <v>310259</v>
       </c>
+      <c r="E44" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1328,12 +1462,15 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Usage And Rates &gt; Home Energy Checkup</t>
+          <t>Usage and Rates &gt; Home Energy Checkup</t>
         </is>
       </c>
       <c r="D45" t="n">
         <v>362420</v>
       </c>
+      <c r="E45" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1348,12 +1485,15 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Usage And Rates &gt; Online Rate Enrollment</t>
+          <t>Usage and Rates &gt; Online Rate Enrollment</t>
         </is>
       </c>
       <c r="D46" t="n">
         <v>140820</v>
       </c>
+      <c r="E46" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1374,6 +1514,9 @@
       <c r="D47" t="n">
         <v>549793</v>
       </c>
+      <c r="E47" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1394,6 +1537,9 @@
       <c r="D48" t="n">
         <v>4516009</v>
       </c>
+      <c r="E48" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1408,12 +1554,15 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Outage &gt; Subscribe Outage (Ew Pages)</t>
+          <t>Outage &gt; Subscribe Outage (EW Pages)</t>
         </is>
       </c>
       <c r="D49" t="n">
         <v>80199</v>
       </c>
+      <c r="E49" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1434,6 +1583,9 @@
       <c r="D50" t="n">
         <v>83947</v>
       </c>
+      <c r="E50" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1454,6 +1606,9 @@
       <c r="D51" t="n">
         <v>137600</v>
       </c>
+      <c r="E51" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1474,6 +1629,9 @@
       <c r="D52" t="n">
         <v>159607</v>
       </c>
+      <c r="E52" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1488,12 +1646,15 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Payment Account New &gt; Create_Payment_Account</t>
+          <t>Payment Account NEW &gt; CREATE_PAYMENT_ACCOUNT</t>
         </is>
       </c>
       <c r="D53" t="n">
         <v>663126</v>
       </c>
+      <c r="E53" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1508,12 +1669,15 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Payment Account New &gt; Update_Payment_Account</t>
+          <t>Payment Account NEW &gt; UPDATE_PAYMENT_ACCOUNT</t>
         </is>
       </c>
       <c r="D54" t="n">
         <v>16176</v>
       </c>
+      <c r="E54" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1528,12 +1692,15 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Payment Account New &gt; Delete_Payment_Account</t>
+          <t>Payment Account NEW &gt; DELETE_PAYMENT_ACCOUNT</t>
         </is>
       </c>
       <c r="D55" t="n">
         <v>244317</v>
       </c>
+      <c r="E55" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1554,6 +1721,9 @@
       <c r="D56" t="n">
         <v>200864</v>
       </c>
+      <c r="E56" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1574,6 +1744,9 @@
       <c r="D57" t="n">
         <v>82019</v>
       </c>
+      <c r="E57" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1594,6 +1767,9 @@
       <c r="D58" t="n">
         <v>178445</v>
       </c>
+      <c r="E58" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1614,6 +1790,9 @@
       <c r="D59" t="n">
         <v>80187</v>
       </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1634,6 +1813,9 @@
       <c r="D60" t="n">
         <v>220049</v>
       </c>
+      <c r="E60" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1654,6 +1836,9 @@
       <c r="D61" t="n">
         <v>79960</v>
       </c>
+      <c r="E61" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1668,12 +1853,15 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Care/Fera</t>
+          <t>CARE/FERA</t>
         </is>
       </c>
       <c r="D62" t="n">
         <v>278569</v>
       </c>
+      <c r="E62" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1694,6 +1882,9 @@
       <c r="D63" t="n">
         <v>302380</v>
       </c>
+      <c r="E63" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1714,6 +1905,9 @@
       <c r="D64" t="n">
         <v>233548</v>
       </c>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1734,6 +1928,9 @@
       <c r="D65" t="n">
         <v>12242</v>
       </c>
+      <c r="E65" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1748,12 +1945,15 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications &gt; Go Paperless Alerts New</t>
+          <t>Alerts &amp; Notifications &gt; Go Paperless Alerts NEW</t>
         </is>
       </c>
       <c r="D66" t="n">
         <v>25758</v>
       </c>
+      <c r="E66" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1768,12 +1968,15 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications &gt; Notices &amp; Services Information New</t>
+          <t>Alerts &amp; Notifications &gt; Notices &amp; Services Information NEW</t>
         </is>
       </c>
       <c r="D67" t="n">
         <v>10738</v>
       </c>
+      <c r="E67" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1788,12 +1991,15 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications &gt; Event Day Alerts New</t>
+          <t>Alerts &amp; Notifications &gt; Event Day Alerts NEW</t>
         </is>
       </c>
       <c r="D68" t="n">
         <v>16104</v>
       </c>
+      <c r="E68" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1808,12 +2014,15 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications &gt; Service Visit Alerts New</t>
+          <t>Alerts &amp; Notifications &gt; Service Visit Alerts NEW</t>
         </is>
       </c>
       <c r="D69" t="n">
         <v>3697</v>
       </c>
+      <c r="E69" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1828,12 +2037,15 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications &gt; Additional Communication Alerts New</t>
+          <t>Alerts &amp; Notifications &gt; Additional Communication Alerts NEW</t>
         </is>
       </c>
       <c r="D70" t="n">
         <v>8686</v>
       </c>
+      <c r="E70" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1848,12 +2060,15 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications &gt; Pay Plan &amp; Shutoff Nonpayment Alerts New</t>
+          <t>Alerts &amp; Notifications &gt; Pay Plan &amp; Shutoff Nonpayment Alerts NEW</t>
         </is>
       </c>
       <c r="D71" t="n">
         <v>16992</v>
       </c>
+      <c r="E71" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1868,12 +2083,15 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Pilot Light Appointments  &gt; Schedule_Service_Appointment</t>
+          <t>Pilot Light Appointments  &gt; SCHEDULE_SERVICE_APPOINTMENT</t>
         </is>
       </c>
       <c r="D72" t="n">
         <v>18987</v>
       </c>
+      <c r="E72" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1888,12 +2106,15 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Pilot Light Appointments  &gt; Reschedule_Service_Appointment</t>
+          <t>Pilot Light Appointments  &gt; RESCHEDULE_SERVICE_APPOINTMENT</t>
         </is>
       </c>
       <c r="D73" t="n">
         <v>1148</v>
       </c>
+      <c r="E73" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1908,12 +2129,15 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Pilot Light Appointments  &gt; Cancel_Service_Appointment</t>
+          <t>Pilot Light Appointments  &gt; CANCEL_SERVICE_APPOINTMENT</t>
         </is>
       </c>
       <c r="D74" t="n">
         <v>1907</v>
       </c>
+      <c r="E74" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1934,6 +2158,9 @@
       <c r="D75" t="n">
         <v>16692</v>
       </c>
+      <c r="E75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1954,6 +2181,9 @@
       <c r="D76" t="n">
         <v>15393</v>
       </c>
+      <c r="E76" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1974,6 +2204,9 @@
       <c r="D77" t="n">
         <v>756747</v>
       </c>
+      <c r="E77" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1993,6 +2226,9 @@
       </c>
       <c r="D78" t="n">
         <v>538774</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>